<commit_message>
added newer version of the ggz zib mappings
</commit_message>
<xml_diff>
--- a/Mappings/FamilySituationChild - STU3.xlsx
+++ b/Mappings/FamilySituationChild - STU3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stijn-nadm\Documents\Mijn docs\git\nictiz-stu3-zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27498" windowHeight="13998" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Voorblad" sheetId="1" r:id="rId1"/>
@@ -594,7 +599,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -781,21 +786,24 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -813,7 +821,13 @@
     <xdr:ext cx="2856900" cy="618995"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -848,7 +862,13 @@
     <xdr:ext cx="1428750" cy="504825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -883,7 +903,13 @@
     <xdr:ext cx="7639050" cy="5076825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -912,7 +938,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -954,7 +980,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -987,9 +1013,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1022,6 +1065,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1202,13 +1262,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1224,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1232,7 +1292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1248,7 +1308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1256,7 +1316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1264,7 +1324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1272,7 +1332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1280,7 +1340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -1288,7 +1348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="90.3" x14ac:dyDescent="0.5">
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
@@ -1296,7 +1356,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
@@ -1304,7 +1364,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
@@ -1312,7 +1372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" ht="51.6" x14ac:dyDescent="0.5">
       <c r="B15" s="2" t="s">
         <v>128</v>
       </c>
@@ -1338,19 +1398,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="19"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1366,7 +1426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1382,7 +1442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1390,7 +1450,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1398,13 +1458,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1412,13 +1472,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1426,13 +1486,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1440,7 +1500,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1448,7 +1508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1456,7 +1516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1464,7 +1524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -1472,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1480,7 +1540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -1488,7 +1548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1496,7 +1556,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -1504,7 +1564,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
@@ -1512,7 +1572,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
@@ -1520,7 +1580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1545,9 +1605,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -1560,11 +1620,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="6" width="2" customWidth="1"/>
@@ -1580,7 +1640,7 @@
     <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
@@ -1620,7 +1680,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B3" s="9" t="s">
         <v>68</v>
       </c>
@@ -1650,7 +1710,7 @@
       </c>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
         <v>73</v>
@@ -1683,12 +1743,12 @@
       <c r="O4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="19" t="s">
         <v>186</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>82</v>
@@ -1717,12 +1777,12 @@
       <c r="O5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="19" t="s">
         <v>185</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B6" s="15"/>
       <c r="C6" s="16" t="s">
         <v>89</v>
@@ -1756,7 +1816,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
@@ -1785,12 +1845,12 @@
       <c r="O7" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P7" s="20" t="s">
+      <c r="P7" s="19" t="s">
         <v>185</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
@@ -1821,12 +1881,12 @@
         <v>104</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="19" t="s">
         <v>185</v>
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
         <v>105</v>
@@ -1855,12 +1915,12 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="20" t="s">
+      <c r="P9" s="19" t="s">
         <v>186</v>
       </c>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B10" s="15"/>
       <c r="C10" s="16" t="s">
         <v>110</v>
@@ -1892,7 +1952,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
@@ -1923,12 +1983,12 @@
       <c r="O11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="19" t="s">
         <v>185</v>
       </c>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13" t="s">
@@ -1959,12 +2019,12 @@
         <v>104</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="19" t="s">
         <v>185</v>
       </c>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B13" s="12"/>
       <c r="C13" s="13" t="s">
         <v>122</v>
@@ -1995,7 +2055,7 @@
         <v>127</v>
       </c>
       <c r="O13" s="2"/>
-      <c r="P13" s="20" t="s">
+      <c r="P13" s="19" t="s">
         <v>188</v>
       </c>
       <c r="Q13" s="2"/>
@@ -2020,7 +2080,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -2029,18 +2089,18 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="19" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.5">
+      <c r="C3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C4" s="18" t="s">
         <v>131</v>
       </c>
@@ -2057,7 +2117,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C5" s="2" t="s">
         <v>136</v>
       </c>
@@ -2074,7 +2134,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C6" s="2" t="s">
         <v>141</v>
       </c>
@@ -2091,7 +2151,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C7" s="2" t="s">
         <v>144</v>
       </c>
@@ -2108,7 +2168,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C8" s="2" t="s">
         <v>147</v>
       </c>
@@ -2125,7 +2185,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C9" s="2" t="s">
         <v>150</v>
       </c>
@@ -2142,7 +2202,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C10" s="2" t="s">
         <v>153</v>
       </c>
@@ -2159,7 +2219,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C11" s="2" t="s">
         <v>156</v>
       </c>
@@ -2176,7 +2236,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C12" s="2" t="s">
         <v>159</v>
       </c>
@@ -2193,7 +2253,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C13" s="2" t="s">
         <v>162</v>
       </c>
@@ -2210,7 +2270,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C14" s="2" t="s">
         <v>165</v>
       </c>
@@ -2227,7 +2287,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C15" s="2" t="s">
         <v>168</v>
       </c>
@@ -2244,7 +2304,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.5">
       <c r="C16" s="2" t="s">
         <v>171</v>
       </c>
@@ -2279,37 +2339,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" ht="154.80000000000001" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" ht="38.700000000000003" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
improvements after review with AH
</commit_message>
<xml_diff>
--- a/Mappings/FamilySituationChild - STU3.xlsx
+++ b/Mappings/FamilySituationChild - STU3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="125">
   <si>
     <t>Concept</t>
   </si>
@@ -390,9 +390,6 @@
   </si>
   <si>
     <t>Observation.component.valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>Observation.extension.reference</t>
   </si>
   <si>
     <t>Observation.component.extension.reference</t>
@@ -606,14 +603,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -922,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1007,7 +1004,7 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="20" t="s">
         <v>117</v>
       </c>
       <c r="Q3" s="4"/>
@@ -1045,14 +1042,14 @@
       <c r="O4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="20" t="s">
         <v>122</v>
       </c>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="2:17" ht="51">
       <c r="B5" s="12"/>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="13"/>
@@ -1079,7 +1076,7 @@
       <c r="O5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="20" t="s">
         <v>123</v>
       </c>
       <c r="Q5" s="2"/>
@@ -1113,8 +1110,8 @@
         <v>35</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="21" t="s">
-        <v>125</v>
+      <c r="P6" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>119</v>
@@ -1149,8 +1146,8 @@
       <c r="O7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="21" t="s">
-        <v>124</v>
+      <c r="P7" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
@@ -1185,7 +1182,7 @@
         <v>45</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>118</v>
       </c>
       <c r="Q8" s="2"/>
@@ -1219,7 +1216,7 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="20" t="s">
         <v>121</v>
       </c>
       <c r="Q9" s="2"/>
@@ -1251,8 +1248,8 @@
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="21" t="s">
-        <v>125</v>
+      <c r="P10" s="20" t="s">
+        <v>124</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>119</v>
@@ -1261,7 +1258,7 @@
     <row r="11" spans="2:17" ht="63.75">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>55</v>
       </c>
       <c r="E11" s="13"/>
@@ -1289,15 +1286,15 @@
       <c r="O11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P11" s="21" t="s">
-        <v>124</v>
+      <c r="P11" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="2:17" ht="25.5">
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>59</v>
       </c>
       <c r="E12" s="13"/>
@@ -1325,7 +1322,7 @@
         <v>45</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="20" t="s">
         <v>118</v>
       </c>
       <c r="Q12" s="2"/>
@@ -1361,7 +1358,7 @@
         <v>68</v>
       </c>
       <c r="O13" s="2"/>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="20" t="s">
         <v>120</v>
       </c>
       <c r="Q13" s="2"/>
@@ -1399,15 +1396,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="18" t="s">

</xml_diff>